<commit_message>
redirect ttd and reminders
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CENPRI\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AC4ED4-5938-45D8-8BBF-2EF523ABADEC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845D3576-E4D5-4B3E-A287-093A278DF937}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -464,15 +464,45 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,36 +522,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -868,7 +868,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:K12"/>
+      <selection activeCell="J16" sqref="J16:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,14 +894,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -909,14 +909,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -924,14 +924,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -939,136 +939,136 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="39"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
       <c r="H7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="22"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="30"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="18">
         <v>43691</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="H8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="31"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="25">
         <v>2</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="29"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1083,17 +1083,17 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="24" t="s">
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="25"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1114,7 +1114,7 @@
       <c r="H14" s="16"/>
       <c r="I14" s="17"/>
       <c r="J14" s="18">
-        <v>43697</v>
+        <v>43693</v>
       </c>
       <c r="K14" s="19"/>
     </row>
@@ -1137,7 +1137,7 @@
       <c r="H15" s="16"/>
       <c r="I15" s="17"/>
       <c r="J15" s="18">
-        <v>43697</v>
+        <v>43694</v>
       </c>
       <c r="K15" s="19"/>
     </row>
@@ -1166,11 +1166,13 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:H3"/>
@@ -1180,16 +1182,14 @@
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C2:H2"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I8:K8"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="C12:K12"/>

</xml_diff>

<commit_message>
pending rfq shortcut to PO
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -2,17 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Department Code" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -86,43 +87,172 @@
     <t xml:space="preserve">  Department:</t>
   </si>
   <si>
-    <t>Test Purchase</t>
-  </si>
-  <si>
-    <t>PR2019-07-09</t>
-  </si>
-  <si>
-    <t>Test Purpose</t>
-  </si>
-  <si>
-    <t>Test Enduse</t>
-  </si>
-  <si>
-    <t>IT Department</t>
-  </si>
-  <si>
-    <t>Stephine</t>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>HR - BCD</t>
+  </si>
+  <si>
+    <t>HRB</t>
+  </si>
+  <si>
+    <t>Billing Department</t>
+  </si>
+  <si>
+    <t>BIL</t>
+  </si>
+  <si>
+    <t>EIC</t>
+  </si>
+  <si>
+    <t>Environment/PCO</t>
+  </si>
+  <si>
+    <t>ENV</t>
+  </si>
+  <si>
+    <t>Finance Department</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>Fuel and Lube Management</t>
+  </si>
+  <si>
+    <t>FLM</t>
+  </si>
+  <si>
+    <t>Health and Safety</t>
+  </si>
+  <si>
+    <t>HAS</t>
+  </si>
+  <si>
+    <t>IT Department - BCD</t>
+  </si>
+  <si>
+    <t>ITB</t>
+  </si>
+  <si>
+    <t>IT Department - SITE</t>
+  </si>
+  <si>
+    <t>ITS</t>
+  </si>
+  <si>
+    <t>Laboratory and Chemical</t>
+  </si>
+  <si>
+    <t>LAB</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>MAI</t>
+  </si>
+  <si>
+    <t>Office of the GM</t>
+  </si>
+  <si>
+    <t>OOG</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>OPE</t>
+  </si>
+  <si>
+    <t>Purchasing Department</t>
+  </si>
+  <si>
+    <t>PUR</t>
+  </si>
+  <si>
+    <t>Reconditioning</t>
+  </si>
+  <si>
+    <t>REC</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>SEC</t>
+  </si>
+  <si>
+    <t>HR - SITE</t>
+  </si>
+  <si>
+    <t>HRS</t>
+  </si>
+  <si>
+    <t>Special Proj/Facilities Imp</t>
+  </si>
+  <si>
+    <t>SPE</t>
+  </si>
+  <si>
+    <t>Trading Department</t>
+  </si>
+  <si>
+    <t>TRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warehouse - CENPRI </t>
+  </si>
+  <si>
+    <t>WHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warehouse - Progen </t>
+  </si>
+  <si>
+    <t>WHP</t>
+  </si>
+  <si>
+    <t>Dept. Code</t>
+  </si>
+  <si>
+    <t>TEST PURCHASE</t>
+  </si>
+  <si>
+    <t>PR-IT</t>
+  </si>
+  <si>
+    <t>Stephine David Severino</t>
+  </si>
+  <si>
+    <t>TEST PURPOSE</t>
+  </si>
+  <si>
+    <t>TEST ENDUSE</t>
   </si>
   <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t>Test Screw</t>
-  </si>
-  <si>
-    <t>Test Hammer</t>
-  </si>
-  <si>
-    <t>Test Ballpen</t>
-  </si>
-  <si>
-    <t>Test Pencil</t>
-  </si>
-  <si>
-    <t>Test Paper</t>
+    <t>Test Mouse</t>
+  </si>
+  <si>
+    <t>Test Keyboard</t>
+  </si>
+  <si>
+    <t>Test Wifi Adapter</t>
   </si>
   <si>
     <t>Test Monitor</t>
+  </si>
+  <si>
+    <t>Test CPU</t>
+  </si>
+  <si>
+    <t>Test Headset</t>
   </si>
 </sst>
 </file>
@@ -132,7 +262,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +289,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,7 +451,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,7 +458,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -329,6 +465,75 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -337,69 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,7 +583,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -738,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,348 +911,378 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="37" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="11"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="38" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="12"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="39" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="12"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="33" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="H7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="29"/>
+      <c r="I7" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="19">
-        <v>43655</v>
-      </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="H8" s="3" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="26">
+        <v>43691</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="H8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="28"/>
-      <c r="K8" s="29"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="H10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="27">
-        <v>2</v>
-      </c>
-      <c r="J9" s="28"/>
-      <c r="K9" s="29"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="8"/>
+      <c r="I10" s="29">
+        <v>1</v>
+      </c>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="29"/>
+      <c r="C11" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="26"/>
+      <c r="C12" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="21" t="s">
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="22"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5">
-        <v>124</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="20"/>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="4">
+        <v>123</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="28"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="B15" s="5">
-        <v>10</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="5">
-        <v>12354</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="20"/>
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1222</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="28"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>3</v>
       </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1312354</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="20"/>
+      <c r="B16" s="4">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="4">
+        <v>13421</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="28"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
-      <c r="B17" s="5">
-        <v>20</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="5">
-        <v>32146</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="20"/>
+      <c r="B17" s="4">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="4">
+        <v>14543</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="28"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>5</v>
       </c>
-      <c r="B18" s="5">
-        <v>15</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="5">
-        <v>234</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="20"/>
+      <c r="B18" s="4">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="4">
+        <v>12424</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>6</v>
       </c>
-      <c r="B19" s="5">
-        <v>4</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="5">
-        <v>36</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="20"/>
+      <c r="B19" s="4">
+        <v>6</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2134</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1112,34 +1290,204 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add checked by in PO, JO and add WH stocks,upload date in PR
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -72,9 +72,6 @@
     <t xml:space="preserve">                      Date Issued:</t>
   </si>
   <si>
-    <t xml:space="preserve">                                PR No.:</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Purpose:</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>TEST PURCHASE</t>
   </si>
   <si>
-    <t>PR-IT</t>
-  </si>
-  <si>
     <t>Stephine David Severino</t>
   </si>
   <si>
@@ -253,6 +247,9 @@
   </si>
   <si>
     <t>Test Headset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       WH Stocks:</t>
   </si>
 </sst>
 </file>
@@ -468,72 +465,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -542,6 +473,72 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,7 +583,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -887,12 +884,12 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:I19"/>
+      <selection activeCell="C11" sqref="C11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -913,14 +910,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -928,14 +925,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -943,14 +940,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -958,102 +955,102 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="29" t="s">
-        <v>64</v>
+      <c r="B7" s="29"/>
+      <c r="C7" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25"/>
       <c r="H7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="25"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="26">
+      <c r="B8" s="29"/>
+      <c r="C8" s="18">
         <v>43691</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="19"/>
       <c r="H8" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>36</v>
+        <v>62</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>35</v>
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="25"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="29" t="s">
-        <v>66</v>
+      <c r="I9" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="29" t="s">
-        <v>65</v>
+      <c r="A10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="23">
+        <v>2</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="25"/>
       <c r="H10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="29">
+        <v>17</v>
+      </c>
+      <c r="I10" s="23">
         <v>1</v>
       </c>
       <c r="J10" s="24"/>
@@ -1062,36 +1059,36 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>67</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
       <c r="G11" s="24"/>
       <c r="H11" s="24"/>
-      <c r="I11" s="30"/>
+      <c r="I11" s="31"/>
       <c r="J11" s="24"/>
       <c r="K11" s="25"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1106,17 +1103,17 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="34" t="s">
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="35"/>
+      <c r="K13" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1126,20 +1123,20 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="4">
         <v>123</v>
       </c>
-      <c r="E14" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="28"/>
+      <c r="E14" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1149,20 +1146,20 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" s="4">
         <v>1222</v>
       </c>
-      <c r="E15" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="28"/>
+      <c r="E15" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1172,20 +1169,20 @@
         <v>3</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="4">
         <v>13421</v>
       </c>
-      <c r="E16" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="28"/>
+      <c r="E16" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -1195,20 +1192,20 @@
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" s="4">
         <v>14543</v>
       </c>
-      <c r="E17" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="28"/>
+      <c r="E17" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -1218,20 +1215,20 @@
         <v>5</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="4">
         <v>12424</v>
       </c>
-      <c r="E18" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="28"/>
+      <c r="E18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -1241,48 +1238,23 @@
         <v>6</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D19" s="4">
         <v>2134</v>
       </c>
-      <c r="E19" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="28"/>
+      <c r="E19" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="E14:I14"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1291,6 +1263,31 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E14:I14"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1313,178 +1310,178 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
         <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
         <v>45</v>
-      </c>
-      <c r="B14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
         <v>47</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
         <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
         <v>57</v>
-      </c>
-      <c r="B20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>59</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pr summary report status -- po issued and partial delivery
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonah\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A194A7-33C9-4469-8359-E7385F976279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -226,12 +227,6 @@
   </si>
   <si>
     <t>keyboard</t>
-  </si>
-  <si>
-    <t>black ink</t>
-  </si>
-  <si>
-    <t>mouse</t>
   </si>
   <si>
     <t>pc/s</t>
@@ -249,7 +244,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -461,10 +456,70 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -472,66 +527,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,7 +571,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -873,11 +868,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:H16"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,14 +899,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -919,14 +914,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -934,14 +929,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -949,134 +944,134 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="17">
+      <c r="B8" s="22"/>
+      <c r="C8" s="28">
         <v>43883</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="18"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
       <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
+      <c r="I9" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="C11" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
+      <c r="C12" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1091,85 +1086,58 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="28"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="4">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="18"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="18"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="23">
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1178,25 +1146,6 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1205,7 +1154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add ,2 in number_format in purchase_order_rev.php
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -226,12 +226,6 @@
   </si>
   <si>
     <t>keyboard</t>
-  </si>
-  <si>
-    <t>black ink</t>
-  </si>
-  <si>
-    <t>mouse</t>
   </si>
   <si>
     <t>pc/s</t>
@@ -461,70 +455,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -532,6 +466,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,7 +570,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -874,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:H16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,14 +898,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -919,14 +913,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -934,14 +928,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -949,134 +943,134 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="31" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="28">
+      <c r="B8" s="30"/>
+      <c r="C8" s="17">
         <v>43883</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="18"/>
       <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
+      <c r="I9" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="C11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
+      <c r="C12" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1091,104 +1085,43 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="28"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="30"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="30"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="30"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
+  <mergeCells count="23">
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1197,6 +1130,21 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add vat in PO
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Stephine enduse</t>
+  </si>
+  <si>
+    <t>mouse</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,70 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -466,66 +529,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,7 +573,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -868,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C12" sqref="C12:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,14 +901,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -913,14 +916,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -928,14 +931,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -943,134 +946,134 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="17">
+      <c r="B8" s="22"/>
+      <c r="C8" s="28">
         <v>43883</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="18"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
       <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1085,19 +1088,19 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="28"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1110,18 +1113,56 @@
         <v>67</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="30"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1130,21 +1171,6 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
will be visible in pending for rfq if po qty incomplete
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonah\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415F8D3B-F9A2-4FBC-8D22-5A8D03EFEB18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,21 +220,12 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>Bacolod</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
     <t>keyboard</t>
   </si>
   <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t>Stephine David</t>
-  </si>
-  <si>
     <t>stephine purpose</t>
   </si>
   <si>
@@ -241,12 +233,21 @@
   </si>
   <si>
     <t>mouse</t>
+  </si>
+  <si>
+    <t>SITE</t>
+  </si>
+  <si>
+    <t>ITSite</t>
+  </si>
+  <si>
+    <t>Jushkyle Jambongana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -458,77 +459,77 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,7 +574,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -870,11 +871,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:K12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,14 +902,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -916,14 +917,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -931,14 +932,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -946,134 +947,134 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="31"/>
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
+      <c r="I7" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="30"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="28">
-        <v>43883</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="19">
+        <v>43984</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="20"/>
       <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="I8" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="31"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
+      <c r="I9" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="31"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
+      <c r="C11" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
+      <c r="C12" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="37"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1088,81 +1089,75 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
       <c r="I13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="39"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="E14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="30"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
+      <c r="E15" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
       <c r="I15" s="16"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="30"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J15:K15"/>
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:H13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1171,6 +1166,12 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1179,7 +1180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Add pr_id in query in pending rfq
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415F8D3B-F9A2-4FBC-8D22-5A8D03EFEB18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,9 +219,6 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>keyboard</t>
-  </si>
-  <si>
     <t>pc/s</t>
   </si>
   <si>
@@ -232,9 +228,6 @@
     <t>Stephine enduse</t>
   </si>
   <si>
-    <t>mouse</t>
-  </si>
-  <si>
     <t>SITE</t>
   </si>
   <si>
@@ -242,12 +235,18 @@
   </si>
   <si>
     <t>Jushkyle Jambongana</t>
+  </si>
+  <si>
+    <t>Screw Driver</t>
+  </si>
+  <si>
+    <t>Monitor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -460,15 +459,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -498,37 +524,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -574,7 +573,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -871,11 +870,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="E15" sqref="E15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,14 +901,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -917,14 +916,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -932,14 +931,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -947,134 +946,134 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="24"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="31"/>
+      <c r="I7" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="19">
+      <c r="B8" s="35"/>
+      <c r="C8" s="20">
         <v>43984</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="20"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="21"/>
       <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="31"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="31"/>
+      <c r="I9" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="18"/>
+      <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="31"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="31"/>
+      <c r="C11" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="37"/>
+      <c r="C12" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1089,40 +1088,40 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="J13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="39"/>
+      <c r="K13" s="28"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
+      <c r="E14" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1132,30 +1131,21 @@
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="E15" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
       <c r="I15" s="16"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="C5:H5"/>
@@ -1172,6 +1162,15 @@
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1180,7 +1179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Change onblur to keyup in price All po form
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F52BF7-4EBF-48FF-8F70-4DABBB8A69AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -220,9 +219,6 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>keyboard</t>
-  </si>
-  <si>
     <t>pc/s</t>
   </si>
   <si>
@@ -241,13 +237,13 @@
     <t>Jushkyle Jambongana</t>
   </si>
   <si>
-    <t>mouse</t>
+    <t>Diesel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -459,52 +455,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -516,12 +473,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,6 +492,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -574,7 +570,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -871,11 +867,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:H15"/>
+      <selection activeCell="A15" sqref="A15:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,14 +898,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -917,14 +913,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -932,14 +928,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -947,134 +943,134 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
+      <c r="I7" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="28">
+      <c r="B8" s="30"/>
+      <c r="C8" s="18">
         <v>43984</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="19"/>
       <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
+      <c r="I9" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="C11" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="37"/>
+      <c r="C12" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1089,60 +1085,64 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="J13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="39"/>
+      <c r="K13" s="28"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="4">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="E14" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="30"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="E14:H14"/>
@@ -1152,21 +1152,6 @@
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:H13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1175,7 +1160,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Fix displaying in pr_report
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-Asus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFBA9548-57B0-4D1A-8FD3-A8B36D2B8C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,35 +220,32 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>stephine purpose</t>
-  </si>
-  <si>
-    <t>Stephine enduse</t>
-  </si>
-  <si>
-    <t>SITE</t>
-  </si>
-  <si>
-    <t>ITSite</t>
-  </si>
-  <si>
-    <t>Jushkyle Jambongana</t>
-  </si>
-  <si>
-    <t>Diesel</t>
+    <t>BCD</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>JASON FLOR</t>
+  </si>
+  <si>
+    <t>SAMPLE</t>
+  </si>
+  <si>
+    <t>PC/S</t>
+  </si>
+  <si>
+    <t>PEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +279,14 @@
     <font>
       <i/>
       <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -431,37 +437,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -469,63 +528,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,10 +569,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -867,267 +869,357 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:K15"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="37" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="38" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="10"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="39" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="10"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="33" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="27">
+        <v>44012</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="H8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="27">
+        <v>44012</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="H9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="26">
+        <v>1</v>
+      </c>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
-      <c r="H7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="24" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="35"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11">
+        <v>5</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="18">
-        <v>43984</v>
-      </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="19"/>
-      <c r="H8" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="26"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="H9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="24" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
-      <c r="H10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="26"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="23"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="28"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4">
-        <v>20</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="19"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="27">
+        <v>44012</v>
+      </c>
+      <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="23">
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1136,35 +1228,21 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="C12:K12"/>
     <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,11 +1250,11 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix export file base from pr_report
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFBA9548-57B0-4D1A-8FD3-A8B36D2B8C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -220,32 +219,35 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>BCD</t>
+    <t>Bacolod</t>
   </si>
   <si>
     <t>IT</t>
   </si>
   <si>
-    <t>JASON FLOR</t>
-  </si>
-  <si>
-    <t>SAMPLE</t>
-  </si>
-  <si>
-    <t>PC/S</t>
-  </si>
-  <si>
-    <t>PEN</t>
+    <t>keyboard</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Stephine David</t>
+  </si>
+  <si>
+    <t>stephine purpose</t>
+  </si>
+  <si>
+    <t>Stephine enduse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,14 +281,6 @@
     <font>
       <i/>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -437,90 +431,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -528,6 +466,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,10 +567,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -869,357 +867,261 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="20" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="5"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="22" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="6"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="22" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="6"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="16" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="H7" s="1" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
+      <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="27">
-        <v>44012</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="H8" s="9" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="17">
+        <v>43883</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="18"/>
+      <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="27">
-        <v>44012</v>
-      </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="H9" s="1" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="H10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="24"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="28"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="25"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-      <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="26">
-        <v>1</v>
-      </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="25"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="33"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="35"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
-        <v>1</v>
-      </c>
-      <c r="B14" s="11">
-        <v>5</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="27">
-        <v>44012</v>
-      </c>
-      <c r="K14" s="29"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1228,21 +1130,34 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C12:K12"/>
     <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,11 +1165,11 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add if not empty statement in purchase request
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Stephine enduse</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>monitor</t>
   </si>
 </sst>
 </file>
@@ -455,10 +461,70 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -466,66 +532,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,7 +576,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -868,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,14 +904,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -913,14 +919,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -928,14 +934,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -943,134 +949,134 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="24" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="17">
+      <c r="B8" s="22"/>
+      <c r="C8" s="28">
         <v>43883</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="18"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
       <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1085,43 +1091,104 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="28"/>
+      <c r="K13" s="37"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="30"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="30"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="27">
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1130,21 +1197,6 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add , 2 in number_format in delivery_reciept
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -222,28 +222,28 @@
     <t>Bacolod</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>keyboard</t>
-  </si>
-  <si>
     <t>pc/s</t>
   </si>
   <si>
-    <t>Stephine David</t>
-  </si>
-  <si>
-    <t>stephine purpose</t>
-  </si>
-  <si>
-    <t>Stephine enduse</t>
-  </si>
-  <si>
-    <t>mouse</t>
-  </si>
-  <si>
-    <t>monitor</t>
+    <t>brromstick</t>
+  </si>
+  <si>
+    <t>dustpan</t>
+  </si>
+  <si>
+    <t>smart diswashing</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Melanie Rocha</t>
+  </si>
+  <si>
+    <t>For cleaning</t>
+  </si>
+  <si>
+    <t>Bcd Office</t>
   </si>
 </sst>
 </file>
@@ -461,70 +461,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -532,6 +472,66 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,7 +576,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -877,7 +877,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E16" sqref="E15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,14 +904,14 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -919,14 +919,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="10"/>
@@ -934,14 +934,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="10"/>
@@ -949,134 +949,136 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="31" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
       <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="27"/>
+      <c r="I7" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="28">
-        <v>43883</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="17">
+        <v>44090</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="18"/>
       <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="27"/>
+      <c r="I8" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
       <c r="H9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="26"/>
-      <c r="K9" s="27"/>
+      <c r="I9" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
       <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="27"/>
+      <c r="I10" s="24">
+        <v>1</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
+      <c r="C11" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="27"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
+      <c r="C12" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1091,19 +1093,19 @@
       <c r="D13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="28"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1113,18 +1115,18 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="16"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="30"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1134,61 +1136,42 @@
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="16"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="30"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="E16" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
       <c r="I16" s="16"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="30"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1197,6 +1180,25 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1209,7 +1211,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
aoq draft - tepen
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CENPRI IT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF836125-315B-4202-B2DC-C8A9D7408AF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -220,31 +219,34 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>Sample Purpose</t>
-  </si>
-  <si>
-    <t>Sample End Use</t>
-  </si>
-  <si>
-    <t>Hand Soap, 100ml</t>
-  </si>
-  <si>
-    <t>bot/s</t>
-  </si>
-  <si>
-    <t>PRMHEC-2021-1002</t>
-  </si>
-  <si>
-    <t>Jason Flor</t>
+    <t>Billing Dept</t>
+  </si>
+  <si>
+    <t>Celina</t>
+  </si>
+  <si>
+    <t>Sample ekk</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>pencil</t>
+  </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>sample</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -575,7 +577,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -872,18 +874,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:K12"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -981,7 +982,7 @@
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25"/>
@@ -1000,7 +1001,7 @@
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="27">
-        <v>44230</v>
+        <v>44229</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
@@ -1008,7 +1009,7 @@
         <v>62</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="25"/>
@@ -1019,7 +1020,7 @@
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="27">
-        <v>44230</v>
+        <v>44237</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="29"/>
@@ -1027,7 +1028,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="25"/>
@@ -1041,9 +1042,7 @@
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="26">
-        <v>3</v>
-      </c>
+      <c r="I10" s="26"/>
       <c r="J10" s="24"/>
       <c r="K10" s="25"/>
     </row>
@@ -1053,7 +1052,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1113,25 +1112,95 @@
         <v>1</v>
       </c>
       <c r="B14" s="11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
-      <c r="I14" s="10">
-        <v>1</v>
-      </c>
+      <c r="I14" s="10"/>
       <c r="J14" s="27">
-        <v>44247</v>
+        <v>43876</v>
       </c>
       <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="11">
+        <v>4</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="27">
+        <v>43877</v>
+      </c>
+      <c r="K15" s="29"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="11">
+        <v>6</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="27">
+        <v>43878</v>
+      </c>
+      <c r="K16" s="29"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
@@ -1160,7 +1229,11 @@
       <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="27">
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:H13"/>
@@ -1192,11 +1265,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
JOI AC COC border
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,40 +219,22 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>BCD</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>Syndey Sinoro</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>roll/s</t>
-  </si>
-  <si>
-    <t>Bacolod Employees</t>
-  </si>
-  <si>
-    <t>Repair broken internet lines</t>
-  </si>
-  <si>
-    <t>box/s</t>
-  </si>
-  <si>
-    <t>UTP Cable</t>
-  </si>
-  <si>
-    <t>RJ 45 Connector Plug</t>
-  </si>
-  <si>
-    <t>Crimping Tool</t>
-  </si>
-  <si>
-    <t>Duct Tape</t>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample2</t>
+  </si>
+  <si>
+    <t>bacolod</t>
+  </si>
+  <si>
+    <t>sample test</t>
+  </si>
+  <si>
+    <t>sample test1</t>
   </si>
 </sst>
 </file>
@@ -295,7 +277,7 @@
     </font>
     <font>
       <i/>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -303,7 +285,7 @@
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -454,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -476,74 +458,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,7 +576,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -886,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,14 +903,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
       <c r="K2" s="5"/>
@@ -930,14 +918,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -945,14 +933,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -960,138 +948,134 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
       <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
+      <c r="I7" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="26">
-        <v>44523</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="17">
+        <v>44548</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="18"/>
       <c r="H8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="24"/>
+      <c r="I8" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="38"/>
+      <c r="K8" s="39"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="26">
-        <v>44523</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="17">
+        <v>44548</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="18"/>
       <c r="H9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="24"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="25">
-        <v>1</v>
-      </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="24"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="24"/>
+      <c r="C11" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="32"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1106,133 +1090,150 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
       <c r="I13" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="J13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="23"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>1</v>
       </c>
       <c r="B14" s="11">
+        <v>30</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="17">
+        <v>44548</v>
+      </c>
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
         <v>2</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="26">
-        <v>44529</v>
-      </c>
-      <c r="K14" s="28"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
-        <v>1</v>
-      </c>
       <c r="B15" s="11">
-        <v>100</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>67</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C15" s="11"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="E15" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="26">
-        <v>44529</v>
-      </c>
-      <c r="K15" s="28"/>
+      <c r="J15" s="17">
+        <v>44548</v>
+      </c>
+      <c r="K15" s="18"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>1</v>
+      <c r="A16" s="10">
+        <v>3</v>
       </c>
       <c r="B16" s="11">
-        <v>1</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>67</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C16" s="11"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
+      <c r="E16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="26">
-        <v>44529</v>
-      </c>
-      <c r="K16" s="28"/>
+      <c r="J16" s="17">
+        <v>44548</v>
+      </c>
+      <c r="K16" s="18"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>1</v>
-      </c>
-      <c r="B17" s="11">
-        <v>10</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>68</v>
-      </c>
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="11"/>
-      <c r="E17" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="26">
-        <v>44529</v>
-      </c>
-      <c r="K17" s="28"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
+  <mergeCells count="37">
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1243,9 +1244,36 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="J20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1255,7 +1283,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change label of Supplier to Contractor in JO Conforme
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SKADA01\Desktop\PR Diesel 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC3BE44-93C5-442B-83E3-F31BCA8CE37C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Department Code" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$K$14</definedName>
-  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -39,6 +37,9 @@
     <t>(Plant Site) Purok San Jose, Barangay Calumangan, Bago City</t>
   </si>
   <si>
+    <t>Telfax: (034) 436-1932</t>
+  </si>
+  <si>
     <t>PURCHASE REQUEST</t>
   </si>
   <si>
@@ -219,32 +220,56 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>Fleur de Liz Ambong / Rey D. Argawanon</t>
-  </si>
-  <si>
-    <t>liters</t>
-  </si>
-  <si>
-    <t>For site's fuel for 5 Engines during commercial operation.</t>
-  </si>
-  <si>
-    <t>Telfax: (034) 435-1932</t>
-  </si>
-  <si>
-    <t>Diesel</t>
-  </si>
-  <si>
-    <t>FDO NO_2022-008</t>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>BCD-ADM</t>
+  </si>
+  <si>
+    <t>Sample Purpose</t>
+  </si>
+  <si>
+    <t>Sample End use</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>Henne</t>
+  </si>
+  <si>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Item 1</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>Item 3</t>
+  </si>
+  <si>
+    <t>Item 4</t>
+  </si>
+  <si>
+    <t>Item 5</t>
+  </si>
+  <si>
+    <t>Item 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +308,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -304,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -424,61 +463,33 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -494,13 +505,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -512,22 +520,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -536,32 +559,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,10 +602,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -903,280 +902,407 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
       <c r="B2" s="15"/>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="29" t="s">
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="29" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="9"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="22" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="27">
+        <v>44750</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="H8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="27">
+        <v>44750</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="H9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="H10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="26"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="35"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11">
+        <v>10</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="11">
+        <v>20</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="29"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
         <v>3</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="33">
-        <v>44676</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="30" t="s">
+      <c r="B16" s="11">
         <v>30</v>
       </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="32"/>
-    </row>
-    <row r="9" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="36">
-        <v>44676</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="6" t="s">
+      <c r="C16" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" s="29"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
         <v>4</v>
       </c>
-      <c r="I9" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="45"/>
-      <c r="K9" s="46"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="37">
-        <v>1</v>
-      </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="32"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="32"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="43"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="B17" s="11">
+        <v>40</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" s="29"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
         <v>5</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B18" s="11">
+        <v>50</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="29"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
         <v>6</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="48"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="21">
-        <v>16000</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B19" s="11">
+        <v>60</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="33">
-        <v>44677</v>
-      </c>
-      <c r="K14" s="35"/>
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="33">
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="E14:H14"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="C9:E9"/>
@@ -1184,6 +1310,7 @@
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1192,201 +1319,203 @@
     <mergeCell ref="C3:H3"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:E7"/>
   </mergeCells>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.45" right="0.45" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="85" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reset series per year
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E073273-F794-4A3B-954F-8893D9BEF275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571115BF-19DD-44F3-B504-0AD868809497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
-  <si>
-    <t>Central Negros Power Reliability, Inc.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>(Main Office) 88 Corner Rizal-Mabini Sts. Bacolod City</t>
   </si>
@@ -223,28 +220,31 @@
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>qw</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>itb</t>
-  </si>
-  <si>
-    <t>henne</t>
-  </si>
-  <si>
-    <t>sample p</t>
-  </si>
-  <si>
-    <t>sample end</t>
+    <t>PROGEN DIESELTECH SERVICES CORP.</t>
+  </si>
+  <si>
+    <t>BCD</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Hennelen</t>
+  </si>
+  <si>
+    <t>Sample Purpose</t>
+  </si>
+  <si>
+    <t>Sample End Use</t>
   </si>
   <si>
     <t>pcs</t>
   </si>
   <si>
-    <t>item 1</t>
+    <t>Item 1</t>
+  </si>
+  <si>
+    <t>Item 2</t>
   </si>
 </sst>
 </file>
@@ -254,7 +254,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,12 +301,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -572,22 +566,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>554522</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>57977</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>505239</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>135372</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -596,7 +590,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -609,8 +603,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19050" y="381000"/>
-          <a:ext cx="1200150" cy="304800"/>
+          <a:off x="554522" y="248477"/>
+          <a:ext cx="563630" cy="657178"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -887,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,7 +909,7 @@
       <c r="A2" s="3"/>
       <c r="B2" s="15"/>
       <c r="C2" s="20" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
@@ -930,7 +924,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
@@ -945,7 +939,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
@@ -960,7 +954,7 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -973,7 +967,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -988,7 +982,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="26" t="s">
@@ -997,7 +991,7 @@
       <c r="D7" s="24"/>
       <c r="E7" s="25"/>
       <c r="H7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="26" t="s">
         <v>66</v>
@@ -1007,38 +1001,38 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="27">
-        <v>44800</v>
+        <v>44930</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
       <c r="H8" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="27">
-        <v>44800</v>
+        <v>44930</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="29"/>
       <c r="H9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="25"/>
@@ -1050,19 +1044,21 @@
       <c r="D10" s="24"/>
       <c r="E10" s="25"/>
       <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="26"/>
+        <v>16</v>
+      </c>
+      <c r="I10" s="26">
+        <v>1</v>
+      </c>
       <c r="J10" s="24"/>
       <c r="K10" s="25"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1076,10 +1072,10 @@
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
@@ -1092,28 +1088,28 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="34" t="s">
         <v>8</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>9</v>
       </c>
       <c r="F13" s="36"/>
       <c r="G13" s="36"/>
       <c r="H13" s="36"/>
       <c r="I13" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K13" s="35"/>
     </row>
@@ -1122,23 +1118,98 @@
         <v>1</v>
       </c>
       <c r="B14" s="11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
       <c r="I14" s="10"/>
       <c r="J14" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="11">
+        <v>10</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="29"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
@@ -1154,7 +1225,9 @@
       <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:H13"/>
@@ -1179,7 +1252,6 @@
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1201,178 +1273,178 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
         <v>48</v>
-      </c>
-      <c r="B16" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
         <v>50</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
         <v>58</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
         <v>60</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed item checker to po qty not delivered qty, PJOR in JOI changed to JO only, changed delivery term in AOQ instead of delivery time
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henne\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonah Benares\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571115BF-19DD-44F3-B504-0AD868809497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10342FDF-CBAB-42AC-AC9A-01B847716047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+  <si>
+    <t>Central Negros Power Reliability, Inc.</t>
+  </si>
   <si>
     <t>(Main Office) 88 Corner Rizal-Mabini Sts. Bacolod City</t>
   </si>
@@ -220,31 +223,22 @@
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>PROGEN DIESELTECH SERVICES CORP.</t>
-  </si>
-  <si>
-    <t>BCD</t>
-  </si>
-  <si>
     <t>IT</t>
   </si>
   <si>
-    <t>Hennelen</t>
+    <t>Jonah Benares</t>
   </si>
   <si>
     <t>Sample Purpose</t>
   </si>
   <si>
-    <t>Sample End Use</t>
-  </si>
-  <si>
-    <t>pcs</t>
-  </si>
-  <si>
-    <t>Item 1</t>
-  </si>
-  <si>
-    <t>Item 2</t>
+    <t>Sample Enduse</t>
+  </si>
+  <si>
+    <t>Sample Item 1</t>
+  </si>
+  <si>
+    <t>sample item 2</t>
   </si>
 </sst>
 </file>
@@ -254,7 +248,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,14 +275,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -446,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -465,8 +451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -490,9 +475,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -502,13 +484,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -566,22 +548,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>554522</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>57977</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>505239</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>135372</xdr:rowOff>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -590,7 +572,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -603,8 +585,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="554522" y="248477"/>
-          <a:ext cx="563630" cy="657178"/>
+          <a:off x="19050" y="381000"/>
+          <a:ext cx="1200150" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -879,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,30 +889,30 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
+      <c r="C3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -938,14 +920,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="C4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -953,281 +935,198 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="C5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
+      <c r="A6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="26" t="s">
+      <c r="A7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
       <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="25">
+        <v>45146</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="27"/>
+      <c r="H8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="22"/>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="25">
+        <v>45146</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="H9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+      <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="25"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="27">
-        <v>44930</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="H8" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="27">
-        <v>44930</v>
-      </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="H9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="25"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-      <c r="H10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="26">
-        <v>1</v>
-      </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="25"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
+        <v>15</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="J13" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="35"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="33"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>1</v>
       </c>
       <c r="B14" s="11">
-        <v>3</v>
-      </c>
-      <c r="C14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="27"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="29"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="10">
-        <v>2</v>
-      </c>
-      <c r="B15" s="11">
-        <v>10</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="K15" s="29"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J15:K15"/>
+  <mergeCells count="23">
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:H13"/>
@@ -1273,178 +1172,178 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix not checking for item balance in repeat order
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonah Benares\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10342FDF-CBAB-42AC-AC9A-01B847716047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -220,13 +219,13 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>YYYY-MM-DD</t>
+    <t>BCD</t>
   </si>
   <si>
     <t>IT</t>
   </si>
   <si>
-    <t>Jonah Benares</t>
+    <t>stephine</t>
   </si>
   <si>
     <t>Sample Purpose</t>
@@ -235,20 +234,23 @@
     <t>Sample Enduse</t>
   </si>
   <si>
-    <t>Sample Item 1</t>
-  </si>
-  <si>
-    <t>sample item 2</t>
+    <t>pc/s</t>
+  </si>
+  <si>
+    <t>Testing Data</t>
+  </si>
+  <si>
+    <t>Aragay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +277,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -432,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -451,7 +461,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,6 +486,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -484,13 +498,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -563,7 +577,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -860,21 +874,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -887,186 +901,188 @@
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="25">
-        <v>45146</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="27">
+        <v>45321</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
       <c r="H8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="22"/>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="25">
-        <v>45146</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="27">
+        <v>45321</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
       <c r="H9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="22"/>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I10" s="26">
+        <v>1</v>
+      </c>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="31"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1079,54 +1095,135 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="13" t="s">
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="33"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K13" s="35"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>1</v>
       </c>
       <c r="B14" s="11">
         <v>10</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="D14" s="11"/>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="27">
+        <v>45327</v>
+      </c>
+      <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="11">
+        <v>15</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" s="27"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>70</v>
-      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="27">
+        <v>45327</v>
+      </c>
+      <c r="K15" s="29"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="25">
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:H13"/>
@@ -1158,19 +1255,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1178,7 +1275,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1186,7 +1283,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1194,7 +1291,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1202,7 +1299,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1210,7 +1307,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1218,7 +1315,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1226,7 +1323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1234,7 +1331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1242,7 +1339,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1250,7 +1347,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1258,7 +1355,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1266,7 +1363,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1274,7 +1371,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1282,7 +1379,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1290,7 +1387,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1298,7 +1395,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -1306,7 +1403,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1314,7 +1411,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1322,7 +1419,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1330,7 +1427,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1338,7 +1435,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
fix JO RFQ ewt for labor and materials
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,28 +219,25 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>BCD</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>stephine</t>
-  </si>
-  <si>
-    <t>Sample Purpose</t>
-  </si>
-  <si>
-    <t>Sample Enduse</t>
-  </si>
-  <si>
-    <t>pc/s</t>
-  </si>
-  <si>
-    <t>Testing Data</t>
-  </si>
-  <si>
-    <t>Aragay</t>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>bcd</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>itb</t>
+  </si>
+  <si>
+    <t>henne</t>
+  </si>
+  <si>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>item 1</t>
   </si>
 </sst>
 </file>
@@ -878,7 +875,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H16" sqref="H16:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,7 +979,7 @@
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25"/>
@@ -1001,7 +998,7 @@
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="27">
-        <v>45321</v>
+        <v>45439</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
@@ -1009,7 +1006,7 @@
         <v>62</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="25"/>
@@ -1020,7 +1017,7 @@
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="27">
-        <v>45321</v>
+        <v>45439</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="29"/>
@@ -1028,7 +1025,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="25"/>
@@ -1054,7 +1051,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1071,7 +1068,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
@@ -1127,33 +1124,23 @@
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="27">
-        <v>45327</v>
+      <c r="J14" s="27" t="s">
+        <v>64</v>
       </c>
       <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>2</v>
-      </c>
-      <c r="B15" s="11">
-        <v>15</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="27">
-        <v>45327</v>
-      </c>
-      <c r="K15" s="29"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
@@ -1221,9 +1208,7 @@
       <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J15:K15"/>
+  <mergeCells count="23">
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:H13"/>

</xml_diff>

<commit_message>
Fix error in vat
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -228,13 +228,22 @@
     <t>itb</t>
   </si>
   <si>
-    <t>henne</t>
-  </si>
-  <si>
     <t>pcs</t>
   </si>
   <si>
     <t>item 1</t>
+  </si>
+  <si>
+    <t>item 2</t>
+  </si>
+  <si>
+    <t>item 3</t>
+  </si>
+  <si>
+    <t>item 4</t>
+  </si>
+  <si>
+    <t>Stephine</t>
   </si>
 </sst>
 </file>
@@ -459,6 +468,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -475,12 +529,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -488,45 +536,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,7 +580,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -871,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,14 +907,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
       <c r="K2" s="5"/>
@@ -913,14 +922,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -928,14 +937,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -943,138 +952,138 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="35"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="28" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="28" t="s">
+      <c r="I7" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="22">
+      <c r="B8" s="21"/>
+      <c r="C8" s="27">
         <v>45439</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="23"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
       <c r="H8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="38" t="s">
+      <c r="I8" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="30"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="22">
+      <c r="B9" s="21"/>
+      <c r="C9" s="27">
         <v>45439</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="23"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
       <c r="H9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="30"/>
+      <c r="I9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="30"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="26">
         <v>1</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="30"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="30"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="18"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1089,19 +1098,19 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K13" s="20"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
@@ -1111,57 +1120,81 @@
         <v>3</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="24" t="s">
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>2</v>
+      </c>
+      <c r="B15" s="11">
+        <v>4</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="23"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="29"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
+      <c r="A16" s="10">
+        <v>3</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
+      <c r="A17" s="10">
+        <v>4</v>
+      </c>
+      <c r="B17" s="11">
+        <v>2</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -1203,7 +1236,26 @@
       <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="29">
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1214,19 +1266,6 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="E14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed regular joi in draft not updating unit price and in revision no vat field
</commit_message>
<xml_diff>
--- a/uploads/excel/PurchaseRequest.xlsx
+++ b/uploads/excel/PurchaseRequest.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GLEN PAUL\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -219,37 +219,31 @@
     <t>WH Stocks</t>
   </si>
   <si>
-    <t>bcd</t>
-  </si>
-  <si>
-    <t>asdasd</t>
-  </si>
-  <si>
-    <t>itb</t>
-  </si>
-  <si>
-    <t>pcs</t>
-  </si>
-  <si>
-    <t>item 1</t>
-  </si>
-  <si>
-    <t>item 2</t>
-  </si>
-  <si>
-    <t>item 3</t>
-  </si>
-  <si>
-    <t>item 4</t>
-  </si>
-  <si>
-    <t>Stephine</t>
+    <t>Airconditioner, Window type Brand: Kolin, Model: KAG-100HME4 Nominal capacity: 1.0 hp Cooling capacity: 9800kJ/h Refrigerant/Charge: R-410A / 460g Power Supply: 1PH / 230V / 60Hz Rated power: 865W Rated current: 3.8 A EER: 11.3</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Manila/Bacolod</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>SCADA ROOM</t>
+  </si>
+  <si>
+    <t>REPLACEMENT OF AIRCONDITIONING UNIT FOR SCADA ROOM</t>
+  </si>
+  <si>
+    <t>GG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -580,7 +574,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -880,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +979,7 @@
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="26" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25"/>
@@ -993,7 +987,7 @@
         <v>18</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="25"/>
@@ -1004,7 +998,7 @@
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="27">
-        <v>45439</v>
+        <v>45498</v>
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
@@ -1012,7 +1006,7 @@
         <v>62</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="25"/>
@@ -1023,7 +1017,7 @@
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="27">
-        <v>45439</v>
+        <v>45498</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="29"/>
@@ -1031,7 +1025,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="25"/>
@@ -1045,9 +1039,7 @@
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="26">
-        <v>1</v>
-      </c>
+      <c r="I10" s="26"/>
       <c r="J10" s="24"/>
       <c r="K10" s="25"/>
     </row>
@@ -1057,7 +1049,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1074,7 +1066,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
@@ -1117,84 +1109,62 @@
         <v>1</v>
       </c>
       <c r="B14" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="37" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="27"/>
+      <c r="J14" s="27">
+        <v>45534</v>
+      </c>
       <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>2</v>
-      </c>
-      <c r="B15" s="11">
-        <v>4</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="29"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
-        <v>3</v>
-      </c>
-      <c r="B16" s="11">
-        <v>1</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="29"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <v>4</v>
-      </c>
-      <c r="B17" s="11">
-        <v>2</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="29"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -1236,13 +1206,7 @@
       <c r="K20" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="J17:K17"/>
+  <mergeCells count="23">
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="E13:H13"/>

</xml_diff>